<commit_message>
Version 8 paper commit
Changes to profile codes and a number of other things based on comments from John, Pat, and Charlotte.
</commit_message>
<xml_diff>
--- a/RLM Cloud Top Pressure Formulas.xlsx
+++ b/RLM Cloud Top Pressure Formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D847B40B-4081-4889-9E66-0C4E36326D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A54CA5-81E9-4D58-9847-9D0B81C12427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C07A726F-92D1-407B-87EB-1C738AC0BD0B}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>L=</t>
   </si>
   <si>
-    <t>m3</t>
-  </si>
-  <si>
     <t>Na=</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>kg of CH4</t>
+  </si>
+  <si>
+    <t>m-3</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
   <dimension ref="A3:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -594,27 +594,27 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4">
         <v>300</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9">
         <v>300</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -625,7 +625,7 @@
         <v>2.687E+25</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
         <v>0</v>
@@ -634,64 +634,72 @@
         <v>2.687E+25</v>
       </c>
       <c r="G10" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="7">
         <v>6.02E+23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" s="3">
         <v>101000</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" s="5">
         <v>2.2000000000000002</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" s="1">
         <v>3.8499999999999999E-27</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="5">
         <f>B12*B16*B11</f>
         <v>2.2249920000000003E-3</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="5">
+        <f>B13</f>
+        <v>2.2249920000000003E-3</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="I13" s="1">
         <f>B10/B11</f>
         <v>44.634551495016609</v>
@@ -699,14 +707,14 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="5">
         <v>1.81E-3</v>
       </c>
       <c r="C14" s="4"/>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" s="1">
         <v>1.81E-3</v>
@@ -714,43 +722,43 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="5">
         <v>22.28</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" s="1">
         <v>22.28</v>
       </c>
       <c r="G15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="5">
         <v>1.6800000000000001E-27</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="1">
         <f>F15*F9*F10*F12/(F14/4)</f>
         <v>1528080.5701657459</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -760,7 +768,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="5">
         <f>B9*B15*B10*B13</f>
@@ -768,7 +776,7 @@
       </c>
       <c r="C18" s="4"/>
       <c r="E18" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="1">
         <f>F9*F15*F10*F12</f>
@@ -783,7 +791,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="5">
         <f>B14*B11</f>
@@ -791,7 +799,7 @@
       </c>
       <c r="C19" s="4"/>
       <c r="E19" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1">
         <f>F14*F11</f>
@@ -801,71 +809,72 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="10">
         <f>B18/B19</f>
         <v>366739.33683977905</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20" s="8">
         <f>F18/F19</f>
         <v>3.7823776489251135</v>
       </c>
       <c r="G20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I20" s="1">
-        <f>I13*F9*F10*F12*F15/(F14*F11)</f>
-        <v>168.82472994454781</v>
+        <f>I13*F9*F13*F15/(F14)</f>
+        <v>366739.33683977905</v>
       </c>
       <c r="J20" s="1">
         <f>I20/F20</f>
-        <v>44.634551495016602</v>
+        <v>96960.000000000015</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="11">
         <f>B20/4</f>
         <v>91684.834209944762</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F21" s="9">
         <f>F20/4</f>
         <v>0.94559441223127838</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I21" s="1">
         <f>I20/4</f>
-        <v>42.206182486136953</v>
+        <v>91684.834209944762</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
+      <c r="I22" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>2.016</v>
@@ -880,7 +889,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>4.0026020000000004</v>
@@ -895,7 +904,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="2">
         <f>SUM(D25:D26)</f>

</xml_diff>